<commit_message>
edited language and write_csv code
</commit_message>
<xml_diff>
--- a/raw data/samplinglist_updated.xlsx
+++ b/raw data/samplinglist_updated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/athellma_ad_unc_edu/Documents/Documents/Duke University/Research/_HBEF/chla/hbef_chla/raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{50E0B27C-21EE-4777-9358-B248CE205576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ECDABC4-3BD1-445F-A94F-C89B760C7B32}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{50E0B27C-21EE-4777-9358-B248CE205576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1DDC0C5-A7B0-414D-B49D-FF0BF9EF718B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9066,8 +9066,8 @@
   <dimension ref="A1:D2691"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2667" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2257" sqref="B2257"/>
+      <pane ySplit="1" topLeftCell="A1526" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1528" sqref="N1528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26410,7 +26410,7 @@
     </row>
     <row r="1544" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1544" s="1">
-        <v>44088</v>
+        <v>44095</v>
       </c>
       <c r="B1544" t="s">
         <v>3</v>
@@ -26421,7 +26421,7 @@
     </row>
     <row r="1545" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1545" s="1">
-        <v>44088</v>
+        <v>44095</v>
       </c>
       <c r="B1545" t="s">
         <v>7</v>
@@ -26432,7 +26432,7 @@
     </row>
     <row r="1546" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1546" s="1">
-        <v>44088</v>
+        <v>44095</v>
       </c>
       <c r="B1546" t="s">
         <v>11</v>
@@ -26443,7 +26443,7 @@
     </row>
     <row r="1547" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1547" s="1">
-        <v>44088</v>
+        <v>44095</v>
       </c>
       <c r="B1547" t="s">
         <v>15</v>
@@ -26454,7 +26454,7 @@
     </row>
     <row r="1548" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1548" s="1">
-        <v>44088</v>
+        <v>44095</v>
       </c>
       <c r="B1548" t="s">
         <v>19</v>
@@ -26465,7 +26465,7 @@
     </row>
     <row r="1549" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1549" s="1">
-        <v>44088</v>
+        <v>44095</v>
       </c>
       <c r="B1549" t="s">
         <v>23</v>
@@ -26476,7 +26476,7 @@
     </row>
     <row r="1550" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1550" s="1">
-        <v>44088</v>
+        <v>44095</v>
       </c>
       <c r="B1550" t="s">
         <v>51</v>

</xml_diff>